<commit_message>
Updated cost and benefit analysis
</commit_message>
<xml_diff>
--- a/Tasks and DRI/Tasks and DRI.xlsx
+++ b/Tasks and DRI/Tasks and DRI.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
   <si>
     <t>Tasks</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Compilation and tidying up of codes</t>
+  </si>
+  <si>
+    <t>Cost and Benefit Analysis</t>
   </si>
 </sst>
 </file>
@@ -437,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,7 +557,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>7</v>
@@ -568,7 +571,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>7</v>
@@ -582,12 +585,26 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>